<commit_message>
Changes with new test cases and framework improved
</commit_message>
<xml_diff>
--- a/src/main/resources/Datasheets/Pillow_Purchase.xlsx
+++ b/src/main/resources/Datasheets/Pillow_Purchase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B971E-7F90-4E21-952E-A1266B03B4FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C88676-E179-4331-BED0-15807FE0B977}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,40 +23,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>operator</t>
-  </si>
-  <si>
-    <t>deepak.n@ab-inbev.com</t>
-  </si>
-  <si>
-    <t>BatchLink</t>
-  </si>
-  <si>
-    <t>lnk_CC001</t>
-  </si>
-  <si>
     <t>Pillow_Purchase</t>
+  </si>
+  <si>
+    <t>CreditCardNumber</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>03/20</t>
+  </si>
+  <si>
+    <t>4811 1111 1111 1114</t>
+  </si>
+  <si>
+    <t>OTP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,14 +65,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,19 +87,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,13 +436,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="10.6328125" customWidth="1"/>
   </cols>
@@ -466,43 +452,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="D2" s="3">
+        <v>123</v>
+      </c>
+      <c r="E2" s="3">
+        <v>112233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D4" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D5E68B16-3AB5-4868-8C28-0FDCB70B8535}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>